<commit_message>
UI Updates - Bug Fixes
</commit_message>
<xml_diff>
--- a/media/resources/ACCOUNT SALE TEMPLATE.xlsx
+++ b/media/resources/ACCOUNT SALE TEMPLATE.xlsx
@@ -847,50 +847,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -925,8 +889,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -953,165 +953,48 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>460375</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>440052</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>67966</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>659334</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>130342</xdr:rowOff>
+      <xdr:rowOff>41757</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4952164" y="0"/>
-          <a:ext cx="4051468" cy="1233237"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" b="1">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>PRIME TEA BROKERS LIMITED</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:effectLst/>
-            <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1st Floor Suite 4, Rex House, Moi Avenue</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>P.O. Box 83070 –80100</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>MOMBASA,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> KENYA</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Tel No. +254 114 591 868</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="r">
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="Arial Nova Cond" panose="020B0506020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>info@primeteabrokers.com</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7683615" y="67966"/>
+          <a:ext cx="2564599" cy="1087132"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1141,7 +1024,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -27336,8 +27219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="68" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27390,22 +27273,22 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="41.25" customHeight="1">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="4"/>
@@ -27470,8 +27353,8 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -27498,70 +27381,70 @@
       <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:16" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="107"/>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121" t="s">
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="116" t="s">
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="122" t="s">
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="124"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="112"/>
     </row>
     <row r="11" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="121"/>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="120">
+      <c r="B11" s="109"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="108">
         <v>44629</v>
       </c>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="118">
+      <c r="F11" s="108"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="106">
         <v>44641</v>
       </c>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="125" t="s">
+      <c r="I11" s="103"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="126"/>
-      <c r="M11" s="126"/>
-      <c r="N11" s="127"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:16" ht="13.5" customHeight="1" thickBot="1">
       <c r="A12" s="15"/>
@@ -27632,8 +27515,8 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="85"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="116"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
@@ -27650,8 +27533,8 @@
       <c r="J15" s="91"/>
       <c r="K15" s="71"/>
       <c r="L15" s="88"/>
-      <c r="M15" s="114"/>
-      <c r="N15" s="114"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="104"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
@@ -27670,8 +27553,8 @@
       <c r="J16" s="91"/>
       <c r="K16" s="75"/>
       <c r="L16" s="94"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="114"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="104"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
@@ -27688,8 +27571,8 @@
       <c r="J17" s="91"/>
       <c r="K17" s="75"/>
       <c r="L17" s="94"/>
-      <c r="M17" s="114"/>
-      <c r="N17" s="114"/>
+      <c r="M17" s="104"/>
+      <c r="N17" s="104"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
@@ -27706,8 +27589,8 @@
       <c r="J18" s="82"/>
       <c r="K18" s="75"/>
       <c r="L18" s="82"/>
-      <c r="M18" s="128"/>
-      <c r="N18" s="128"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
@@ -27741,11 +27624,11 @@
         <f>SUM(L15:L18)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="110">
+      <c r="M19" s="121">
         <f>SUM(M15:M18)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="110"/>
+      <c r="N19" s="121"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
@@ -27764,8 +27647,8 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="L20" s="73"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="112"/>
+      <c r="M20" s="123"/>
+      <c r="N20" s="123"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
@@ -27786,8 +27669,8 @@
       <c r="J21" s="39"/>
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="113"/>
+      <c r="M21" s="124"/>
+      <c r="N21" s="124"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
@@ -27816,8 +27699,8 @@
       <c r="J22" s="39"/>
       <c r="K22" s="39"/>
       <c r="L22" s="39"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="113"/>
+      <c r="M22" s="124"/>
+      <c r="N22" s="124"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
@@ -27851,8 +27734,8 @@
       <c r="J23" s="45"/>
       <c r="K23" s="45"/>
       <c r="L23" s="45"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="111"/>
+      <c r="M23" s="122"/>
+      <c r="N23" s="122"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
@@ -27873,11 +27756,11 @@
       <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="L24" s="49"/>
-      <c r="M24" s="110">
+      <c r="M24" s="121">
         <f>M19-M23</f>
         <v>0</v>
       </c>
-      <c r="N24" s="110"/>
+      <c r="N24" s="121"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
@@ -27894,8 +27777,8 @@
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
       <c r="L25" s="50"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
+      <c r="M25" s="117"/>
+      <c r="N25" s="117"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
@@ -27916,8 +27799,8 @@
       <c r="J26" s="36"/>
       <c r="K26" s="54"/>
       <c r="L26" s="54"/>
-      <c r="M26" s="108"/>
-      <c r="N26" s="108"/>
+      <c r="M26" s="118"/>
+      <c r="N26" s="118"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
@@ -27934,8 +27817,8 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
+      <c r="M27" s="119"/>
+      <c r="N27" s="119"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
@@ -27952,8 +27835,8 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="104"/>
-      <c r="N28" s="104"/>
+      <c r="M28" s="120"/>
+      <c r="N28" s="120"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
@@ -27970,8 +27853,8 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="104"/>
-      <c r="N29" s="104"/>
+      <c r="M29" s="120"/>
+      <c r="N29" s="120"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
@@ -27988,8 +27871,8 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="104"/>
-      <c r="N30" s="104"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
@@ -28006,8 +27889,8 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="104"/>
-      <c r="N31" s="104"/>
+      <c r="M31" s="120"/>
+      <c r="N31" s="120"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
@@ -28024,8 +27907,8 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
+      <c r="M32" s="127"/>
+      <c r="N32" s="127"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
@@ -28042,8 +27925,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="103"/>
-      <c r="N33" s="103"/>
+      <c r="M33" s="127"/>
+      <c r="N33" s="127"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
@@ -28060,8 +27943,8 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="105"/>
-      <c r="N34" s="105"/>
+      <c r="M34" s="128"/>
+      <c r="N34" s="128"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
@@ -28082,10 +27965,10 @@
       <c r="J35" s="65"/>
       <c r="K35" s="65"/>
       <c r="L35" s="65"/>
-      <c r="M35" s="102" t="s">
+      <c r="M35" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="102"/>
+      <c r="N35" s="126"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
@@ -28102,8 +27985,8 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="103"/>
-      <c r="N36" s="103"/>
+      <c r="M36" s="127"/>
+      <c r="N36" s="127"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
@@ -28120,8 +28003,8 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="103"/>
-      <c r="N37" s="103"/>
+      <c r="M37" s="127"/>
+      <c r="N37" s="127"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
@@ -28165,6 +28048,28 @@
     <row r="51" ht="21.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M28:N28"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="M15:N15"/>
@@ -28178,28 +28083,6 @@
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M34:N34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.17" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement Account Sales | Update Checker | Better Management of Generated Files
</commit_message>
<xml_diff>
--- a/media/resources/ACCOUNT SALE TEMPLATE.xlsx
+++ b/media/resources/ACCOUNT SALE TEMPLATE.xlsx
@@ -162,7 +162,7 @@
     <t>PRME/22/010</t>
   </si>
   <si>
-    <t>PROMPT DATE</t>
+    <t>PROMPT  DATE</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -847,6 +847,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,6 +895,24 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -904,29 +925,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11967,62 +11980,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="219075"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="233" name="Text Box 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80B0D492-4E97-4589-835E-672179B18A2F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="857250" y="5667375"/>
-          <a:ext cx="76200" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -15719,62 +15676,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="219075"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="300" name="Text Box 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED60AE5-64DA-4D17-A751-3EDA67C270BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="933450" y="5705475"/>
-          <a:ext cx="76200" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -17007,118 +16908,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="323" name="Text Box 286">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B521B87-5278-4565-98D3-20E1567D1767}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="5867400"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="324" name="Text Box 300">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E192C5-DE6A-49D6-BCF2-BA82C9182810}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1038225" y="6496050"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -17175,230 +16964,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="326" name="Text Box 257">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F6E2431-9ECB-4E7E-95EA-364E36AE21FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="327" name="Text Box 271">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38621CF5-90D1-4DF7-9061-8E57DFDD9196}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="328" name="Text Box 286">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{684ECEFA-ADD5-4B9D-9DC5-FC54FF62F6B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="329" name="Text Box 300">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{366955F1-5F9F-4A17-AA33-72AB65F15A76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -17455,230 +17020,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="331" name="Text Box 257">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F486FA4-8A23-4E5B-84DF-C1767ED886EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="332" name="Text Box 271">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D75D5C-4C2F-4ADC-A51F-B96241635325}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="333" name="Text Box 286">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53CDFC69-BB9E-472E-8349-06DADE6ACBA4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="334" name="Text Box 300">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34CB90EB-0BF7-4BBC-9A9C-3BB30FC592E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -17701,118 +17042,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="57150" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="336" name="Text Box 257">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148FF1D9-76E0-4C0F-94E3-F74CCDC059E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="847725" y="6143625"/>
-          <a:ext cx="76200" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393326</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="337" name="Text Box 271">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0842909B-A5D7-4A95-AC09-2B10A6DBC1CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1267385" y="6129617"/>
           <a:ext cx="76200" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -27217,10 +26446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P200"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27273,22 +26502,22 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="41.25" customHeight="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="4"/>
@@ -27353,8 +26582,8 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -27381,70 +26610,70 @@
       <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:16" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="107"/>
-      <c r="K9" s="107"/>
-      <c r="L9" s="107"/>
-      <c r="M9" s="107"/>
-      <c r="N9" s="107"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="109"/>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109" t="s">
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="103" t="s">
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="110" t="s">
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="111"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="113"/>
     </row>
     <row r="11" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="109"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="108">
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="109">
         <v>44629</v>
       </c>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="106">
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="107">
         <v>44641</v>
       </c>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="113" t="s">
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="114"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="115"/>
+      <c r="N11" s="116"/>
     </row>
     <row r="12" spans="1:16" ht="13.5" customHeight="1" thickBot="1">
       <c r="A12" s="15"/>
@@ -27515,8 +26744,8 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="85"/>
-      <c r="M14" s="116"/>
-      <c r="N14" s="116"/>
+      <c r="M14" s="117"/>
+      <c r="N14" s="117"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
@@ -27533,8 +26762,8 @@
       <c r="J15" s="91"/>
       <c r="K15" s="71"/>
       <c r="L15" s="88"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
@@ -27553,26 +26782,26 @@
       <c r="J16" s="91"/>
       <c r="K16" s="75"/>
       <c r="L16" s="94"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A17" s="86"/>
+      <c r="A17" s="95"/>
       <c r="B17" s="86"/>
       <c r="C17" s="86"/>
       <c r="D17" s="86"/>
       <c r="E17" s="86"/>
       <c r="F17" s="87"/>
-      <c r="G17" s="94"/>
+      <c r="G17" s="102"/>
       <c r="H17" s="84"/>
       <c r="I17" s="72"/>
       <c r="J17" s="91"/>
       <c r="K17" s="75"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="104"/>
-      <c r="N17" s="104"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
@@ -27589,8 +26818,8 @@
       <c r="J18" s="82"/>
       <c r="K18" s="75"/>
       <c r="L18" s="82"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="125"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="119"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
@@ -27624,11 +26853,11 @@
         <f>SUM(L15:L18)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="121">
+      <c r="M19" s="118">
         <f>SUM(M15:M18)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="121"/>
+      <c r="N19" s="118"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
@@ -27647,8 +26876,8 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="L20" s="73"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="123"/>
+      <c r="M20" s="122"/>
+      <c r="N20" s="122"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
@@ -27669,8 +26898,8 @@
       <c r="J21" s="39"/>
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
-      <c r="M21" s="124"/>
-      <c r="N21" s="124"/>
+      <c r="M21" s="123"/>
+      <c r="N21" s="123"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
@@ -27688,7 +26917,7 @@
       <c r="E22" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="130" t="s">
         <v>29</v>
       </c>
       <c r="G22" s="43"/>
@@ -27699,8 +26928,8 @@
       <c r="J22" s="39"/>
       <c r="K22" s="39"/>
       <c r="L22" s="39"/>
-      <c r="M22" s="124"/>
-      <c r="N22" s="124"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="123"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
@@ -27734,8 +26963,8 @@
       <c r="J23" s="45"/>
       <c r="K23" s="45"/>
       <c r="L23" s="45"/>
-      <c r="M23" s="122"/>
-      <c r="N23" s="122"/>
+      <c r="M23" s="121"/>
+      <c r="N23" s="121"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
@@ -27756,11 +26985,11 @@
       <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="L24" s="49"/>
-      <c r="M24" s="121">
+      <c r="M24" s="118">
         <f>M19-M23</f>
         <v>0</v>
       </c>
-      <c r="N24" s="121"/>
+      <c r="N24" s="118"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
@@ -27772,13 +27001,13 @@
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
       <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="H25" s="132"/>
       <c r="I25" s="50"/>
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
       <c r="L25" s="50"/>
-      <c r="M25" s="117"/>
-      <c r="N25" s="117"/>
+      <c r="M25" s="124"/>
+      <c r="N25" s="124"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
@@ -27799,8 +27028,8 @@
       <c r="J26" s="36"/>
       <c r="K26" s="54"/>
       <c r="L26" s="54"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="125"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
@@ -27817,8 +27046,8 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="119"/>
-      <c r="N27" s="119"/>
+      <c r="M27" s="126"/>
+      <c r="N27" s="126"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
@@ -27835,8 +27064,8 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="120"/>
-      <c r="N28" s="120"/>
+      <c r="M28" s="131"/>
+      <c r="N28" s="131"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
@@ -27847,14 +27076,14 @@
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
       <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
+      <c r="G29" s="133"/>
       <c r="H29" s="59"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="120"/>
-      <c r="N29" s="120"/>
+      <c r="M29" s="127"/>
+      <c r="N29" s="127"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
@@ -27871,8 +27100,8 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="120"/>
-      <c r="N30" s="120"/>
+      <c r="M30" s="127"/>
+      <c r="N30" s="127"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
@@ -27889,8 +27118,8 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="120"/>
-      <c r="N31" s="120"/>
+      <c r="M31" s="127"/>
+      <c r="N31" s="127"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
@@ -27907,8 +27136,8 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="127"/>
-      <c r="N32" s="127"/>
+      <c r="M32" s="128"/>
+      <c r="N32" s="128"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
@@ -27925,8 +27154,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="127"/>
-      <c r="N33" s="127"/>
+      <c r="M33" s="128"/>
+      <c r="N33" s="128"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
@@ -27943,8 +27172,8 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="128"/>
-      <c r="N34" s="128"/>
+      <c r="M34" s="129"/>
+      <c r="N34" s="129"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
@@ -27965,10 +27194,10 @@
       <c r="J35" s="65"/>
       <c r="K35" s="65"/>
       <c r="L35" s="65"/>
-      <c r="M35" s="126" t="s">
+      <c r="M35" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="126"/>
+      <c r="N35" s="120"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
@@ -27985,8 +27214,8 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="127"/>
-      <c r="N36" s="127"/>
+      <c r="M36" s="128"/>
+      <c r="N36" s="128"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
@@ -28003,8 +27232,8 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="127"/>
-      <c r="N37" s="127"/>
+      <c r="M37" s="128"/>
+      <c r="N37" s="128"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
@@ -28028,26 +27257,175 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" ht="21.75" customHeight="1">
+    <row r="43" spans="1:16" ht="19.8" customHeight="1">
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" ht="21.75" hidden="1" customHeight="1">
+    <row r="44" spans="1:16" ht="21.75" customHeight="1">
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" ht="21.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:16" ht="21.75" customHeight="1">
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" ht="21.75" hidden="1" customHeight="1"/>
+    <row r="46" spans="1:16" ht="21.75" customHeight="1"/>
     <row r="47" spans="1:16" ht="21.75" customHeight="1"/>
     <row r="48" spans="1:16" ht="21.75" customHeight="1"/>
     <row r="49" ht="21.75" customHeight="1"/>
     <row r="50" ht="21.75" customHeight="1"/>
     <row r="51" ht="21.75" customHeight="1"/>
+    <row r="52" ht="21.75" customHeight="1"/>
+    <row r="53" ht="21.75" customHeight="1"/>
+    <row r="54" ht="21.75" customHeight="1"/>
+    <row r="55" ht="21.75" customHeight="1"/>
+    <row r="56" ht="21.75" customHeight="1"/>
+    <row r="57" ht="21.75" customHeight="1"/>
+    <row r="58" ht="21.75" customHeight="1"/>
+    <row r="59" ht="21.75" customHeight="1"/>
+    <row r="60" ht="21.75" customHeight="1"/>
+    <row r="61" ht="21.75" customHeight="1"/>
+    <row r="62" ht="21.75" customHeight="1"/>
+    <row r="63" ht="21.75" customHeight="1"/>
+    <row r="64" ht="21.75" customHeight="1"/>
+    <row r="65" ht="21.75" customHeight="1"/>
+    <row r="66" ht="21.75" customHeight="1"/>
+    <row r="67" ht="21.75" customHeight="1"/>
+    <row r="68" ht="21.75" customHeight="1"/>
+    <row r="69" ht="21.75" customHeight="1"/>
+    <row r="70" ht="21.75" customHeight="1"/>
+    <row r="71" ht="21.75" customHeight="1"/>
+    <row r="72" ht="21.75" customHeight="1"/>
+    <row r="73" ht="21.75" customHeight="1"/>
+    <row r="74" ht="21.75" customHeight="1"/>
+    <row r="75" ht="21.75" customHeight="1"/>
+    <row r="76" ht="21.75" customHeight="1"/>
+    <row r="77" ht="21.75" customHeight="1"/>
+    <row r="78" ht="21.75" customHeight="1"/>
+    <row r="79" ht="21.75" customHeight="1"/>
+    <row r="80" ht="21.75" customHeight="1"/>
+    <row r="81" ht="21.75" customHeight="1"/>
+    <row r="82" ht="21.75" customHeight="1"/>
+    <row r="83" ht="21.75" customHeight="1"/>
+    <row r="84" ht="21.75" customHeight="1"/>
+    <row r="85" ht="21.75" customHeight="1"/>
+    <row r="86" ht="21.75" customHeight="1"/>
+    <row r="87" ht="21.75" customHeight="1"/>
+    <row r="88" ht="21.75" customHeight="1"/>
+    <row r="89" ht="21.75" customHeight="1"/>
+    <row r="90" ht="21.75" customHeight="1"/>
+    <row r="91" ht="21.75" customHeight="1"/>
+    <row r="92" ht="21.75" customHeight="1"/>
+    <row r="93" ht="21.75" customHeight="1"/>
+    <row r="94" ht="21.75" customHeight="1"/>
+    <row r="95" ht="21.75" customHeight="1"/>
+    <row r="96" ht="21.75" customHeight="1"/>
+    <row r="97" ht="21.75" customHeight="1"/>
+    <row r="98" ht="21.75" customHeight="1"/>
+    <row r="99" ht="21.75" customHeight="1"/>
+    <row r="100" ht="21.75" customHeight="1"/>
+    <row r="101" ht="21.75" customHeight="1"/>
+    <row r="102" ht="21.75" customHeight="1"/>
+    <row r="103" ht="21.75" customHeight="1"/>
+    <row r="104" ht="21.75" customHeight="1"/>
+    <row r="105" ht="21.75" customHeight="1"/>
+    <row r="106" ht="21.75" customHeight="1"/>
+    <row r="107" ht="21.75" customHeight="1"/>
+    <row r="108" ht="21.75" customHeight="1"/>
+    <row r="109" ht="21.75" customHeight="1"/>
+    <row r="110" ht="21.75" customHeight="1"/>
+    <row r="111" ht="21.75" customHeight="1"/>
+    <row r="112" ht="21.75" customHeight="1"/>
+    <row r="113" ht="21.75" customHeight="1"/>
+    <row r="114" ht="21.75" customHeight="1"/>
+    <row r="115" ht="21.75" customHeight="1"/>
+    <row r="116" ht="21.75" customHeight="1"/>
+    <row r="117" ht="21.75" customHeight="1"/>
+    <row r="118" ht="21.75" customHeight="1"/>
+    <row r="119" ht="21.75" customHeight="1"/>
+    <row r="120" ht="21.75" customHeight="1"/>
+    <row r="121" ht="21.75" customHeight="1"/>
+    <row r="122" ht="21.75" customHeight="1"/>
+    <row r="123" ht="21.75" customHeight="1"/>
+    <row r="124" ht="21.75" customHeight="1"/>
+    <row r="125" ht="21.75" customHeight="1"/>
+    <row r="126" ht="21.75" customHeight="1"/>
+    <row r="127" ht="21.75" customHeight="1"/>
+    <row r="128" ht="21.75" customHeight="1"/>
+    <row r="129" ht="21.75" customHeight="1"/>
+    <row r="130" ht="21.75" customHeight="1"/>
+    <row r="131" ht="21.75" customHeight="1"/>
+    <row r="132" ht="21.75" customHeight="1"/>
+    <row r="133" ht="21.75" customHeight="1"/>
+    <row r="134" ht="21.75" customHeight="1"/>
+    <row r="135" ht="21.75" customHeight="1"/>
+    <row r="136" ht="21.75" customHeight="1"/>
+    <row r="137" ht="21.75" customHeight="1"/>
+    <row r="138" ht="21.75" customHeight="1"/>
+    <row r="139" ht="21.75" customHeight="1"/>
+    <row r="140" ht="21.75" customHeight="1"/>
+    <row r="141" ht="21.75" customHeight="1"/>
+    <row r="142" ht="21.75" customHeight="1"/>
+    <row r="143" ht="21.75" customHeight="1"/>
+    <row r="144" ht="21.75" customHeight="1"/>
+    <row r="145" ht="21.75" customHeight="1"/>
+    <row r="146" ht="21.75" customHeight="1"/>
+    <row r="147" ht="21.75" customHeight="1"/>
+    <row r="148" ht="21.75" customHeight="1"/>
+    <row r="149" ht="21.75" customHeight="1"/>
+    <row r="150" ht="21.75" customHeight="1"/>
+    <row r="151" ht="21.75" customHeight="1"/>
+    <row r="152" ht="21.75" customHeight="1"/>
+    <row r="153" ht="21.75" customHeight="1"/>
+    <row r="154" ht="21.75" customHeight="1"/>
+    <row r="155" ht="21.75" customHeight="1"/>
+    <row r="156" ht="21.75" customHeight="1"/>
+    <row r="157" ht="21.75" customHeight="1"/>
+    <row r="158" ht="21.75" customHeight="1"/>
+    <row r="159" ht="21.75" customHeight="1"/>
+    <row r="160" ht="21.75" customHeight="1"/>
+    <row r="161" ht="21.75" customHeight="1"/>
+    <row r="162" ht="21.75" customHeight="1"/>
+    <row r="163" ht="21.75" customHeight="1"/>
+    <row r="164" ht="21.75" customHeight="1"/>
+    <row r="165" ht="21.75" customHeight="1"/>
+    <row r="166" ht="21.75" customHeight="1"/>
+    <row r="167" ht="21.75" customHeight="1"/>
+    <row r="168" ht="21.75" customHeight="1"/>
+    <row r="169" ht="21.75" customHeight="1"/>
+    <row r="170" ht="21.75" customHeight="1"/>
+    <row r="171" ht="21.75" customHeight="1"/>
+    <row r="172" ht="21.75" customHeight="1"/>
+    <row r="173" ht="21.75" customHeight="1"/>
+    <row r="174" ht="21.75" customHeight="1"/>
+    <row r="175" ht="21.75" customHeight="1"/>
+    <row r="176" ht="21.75" customHeight="1"/>
+    <row r="177" ht="21.75" customHeight="1"/>
+    <row r="178" ht="21.75" customHeight="1"/>
+    <row r="179" ht="21.75" customHeight="1"/>
+    <row r="180" ht="21.75" customHeight="1"/>
+    <row r="181" ht="21.75" customHeight="1"/>
+    <row r="182" ht="21.75" customHeight="1"/>
+    <row r="183" ht="21.75" customHeight="1"/>
+    <row r="184" ht="21.75" customHeight="1"/>
+    <row r="185" ht="21.75" customHeight="1"/>
+    <row r="186" ht="21.75" customHeight="1"/>
+    <row r="187" ht="21.75" customHeight="1"/>
+    <row r="188" ht="21.75" customHeight="1"/>
+    <row r="189" ht="21.75" customHeight="1"/>
+    <row r="190" ht="21.75" customHeight="1"/>
+    <row r="191" ht="21.75" customHeight="1"/>
+    <row r="192" ht="21.75" customHeight="1"/>
+    <row r="193" ht="21.75" customHeight="1"/>
+    <row r="194" ht="21.75" customHeight="1"/>
+    <row r="195" ht="21.75" customHeight="1"/>
+    <row r="196" ht="21.75" customHeight="1"/>
+    <row r="197" ht="21.75" customHeight="1"/>
+    <row r="198" ht="21.75" customHeight="1"/>
+    <row r="199" ht="21.75" customHeight="1"/>
+    <row r="200" ht="21.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="34">
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="M30:N30"/>
@@ -28056,7 +27434,6 @@
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M35:N35"/>

</xml_diff>